<commit_message>
Comments in Config file
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UIPath\FaceRecognitionML\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D353AF-BC8C-44E0-B0B0-9975812959BA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1090A7BC-2626-48C1-A275-BCBACAEF8406}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
   <si>
     <t>Name</t>
   </si>
@@ -152,6 +152,15 @@
   </si>
   <si>
     <t>D:\UIPath\FaceRecognitionML\Python\TensorFlowModel\dict.txt</t>
+  </si>
+  <si>
+    <t>Complete Path</t>
+  </si>
+  <si>
+    <t>Relative Path</t>
+  </si>
+  <si>
+    <t>Anaconda Environment Py3_TF =&gt; Tensorflow 2.3.0 || Numpy 1.20.1 || Pillow 8.2.0 (dif vers may have compat Issues)</t>
   </si>
 </sst>
 </file>
@@ -183,12 +192,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -203,7 +218,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -213,6 +228,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -529,15 +545,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="43.5703125" customWidth="1"/>
-    <col min="2" max="2" width="57.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="2" max="2" width="65" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="105.140625" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -601,42 +617,57 @@
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" t="s">
-        <v>32</v>
+        <v>37</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
         <v>34</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="5" t="s">
         <v>39</v>
+      </c>
+      <c r="C8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
         <v>35</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="5" t="s">
         <v>40</v>
+      </c>
+      <c r="C9" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
         <v>36</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="5" t="s">
         <v>41</v>
+      </c>
+      <c r="C10" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>